<commit_message>
Add additional clean sample data for Power BI
</commit_message>
<xml_diff>
--- a/powerbi/LearningPlatform_Data.xlsx
+++ b/powerbi/LearningPlatform_Data.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,6 +573,116 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>2024-03-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>L006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>frank@example.com</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-03-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>L007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>grace@example.com</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-03-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>L008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>harry@example.com</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-03-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>L009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>irene@example.com</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-03-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>L010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>jack@example.com</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
         </is>
       </c>
     </row>
@@ -587,7 +697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -838,6 +948,346 @@
         <v>0</v>
       </c>
       <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>E007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>L006</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>C101</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>I001</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="F8" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" t="n">
+        <v>60</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>E008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>L006</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>C105</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>I003</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45373</v>
+      </c>
+      <c r="F9" t="n">
+        <v>40</v>
+      </c>
+      <c r="G9" t="n">
+        <v>120</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>E009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>L007</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>C102</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>I002</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="F10" t="n">
+        <v>60</v>
+      </c>
+      <c r="G10" t="n">
+        <v>180</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>E010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>L007</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>C105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>I003</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45376</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" t="n">
+        <v>45</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>E011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>L008</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>C103</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>I001</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45377</v>
+      </c>
+      <c r="F12" t="n">
+        <v>80</v>
+      </c>
+      <c r="G12" t="n">
+        <v>300</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>E012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>L009</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>C106</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>I004</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>45380</v>
+      </c>
+      <c r="F13" t="n">
+        <v>30</v>
+      </c>
+      <c r="G13" t="n">
+        <v>90</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>E013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>L009</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>C107</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>I004</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>E014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>L010</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>C108</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>I004</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>45384</v>
+      </c>
+      <c r="F15" t="n">
+        <v>15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>75</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>E015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>L010</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>C101</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>I001</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>45387</v>
+      </c>
+      <c r="F16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" t="n">
+        <v>200</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>E016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>L005</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>C105</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>I003</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="F17" t="n">
+        <v>30</v>
+      </c>
+      <c r="G17" t="n">
+        <v>100</v>
+      </c>
+      <c r="H17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -852,7 +1302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -985,6 +1435,106 @@
       </c>
       <c r="E5" t="n">
         <v>540</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C105</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Data Visualization with Power BI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C106</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Advanced SQL Optimization</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>C107</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cloud Data Warehousing with Snowflake</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>C108</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Kafka &amp; Spark</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -998,7 +1548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1390,6 +1940,546 @@
       </c>
       <c r="L7" t="n">
         <v>600</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>E007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>L006</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>C101</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>I001</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-03-18</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" t="n">
+        <v>60</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Data Engineering Fundamentals</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>E008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>L006</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>C105</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>I003</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-03-22</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>40</v>
+      </c>
+      <c r="G9" t="n">
+        <v>120</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Data Visualization with Power BI</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>E009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>L007</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>C102</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>I002</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-03-23</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>60</v>
+      </c>
+      <c r="G10" t="n">
+        <v>180</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Machine Learning Basics</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>E010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>L007</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>C105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>I003</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-03-25</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" t="n">
+        <v>45</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Data Visualization with Power BI</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>E011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>L008</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>C103</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>I001</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-03-26</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>80</v>
+      </c>
+      <c r="G12" t="n">
+        <v>300</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>SQL for Analytics</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>E012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>L009</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>C106</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>I004</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-03-29</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>30</v>
+      </c>
+      <c r="G13" t="n">
+        <v>90</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Advanced SQL Optimization</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>E013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>L009</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>C107</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>I004</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-03-30</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Cloud Data Warehousing with Snowflake</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>E014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>L010</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>C108</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>I004</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2024-04-02</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>75</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Kafka &amp; Spark</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>E015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>L010</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>C101</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>I001</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2024-04-05</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" t="n">
+        <v>200</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Data Engineering Fundamentals</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>E016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>L005</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>C105</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>I003</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2024-03-18</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>30</v>
+      </c>
+      <c r="G17" t="n">
+        <v>100</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Data Visualization with Power BI</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Data Science</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -1403,7 +2493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1468,6 +2558,78 @@
         <v>45363</v>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45373</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45376</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45377</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45380</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45384</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45387</v>
+      </c>
+      <c r="B16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1482,7 +2644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1505,31 +2667,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Data Engineering Fundamentals</t>
+          <t>Advanced SQL Optimization</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Machine Learning Basics</t>
+          <t>Cloud Data Warehousing with Snowflake</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Data Engineering Fundamentals</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Data Visualization with Power BI</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Machine Learning Basics</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Kafka &amp; Spark</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>SQL for Analytics</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
+      <c r="B8" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1570,7 +2772,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -1580,7 +2782,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1594,7 +2796,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1622,40 +2824,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Data Engineering Fundamentals</t>
+          <t>Advanced SQL Optimization</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>83.33333333333333</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Machine Learning Basics</t>
+          <t>Cloud Data Warehousing with Snowflake</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>37.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Data Engineering Fundamentals</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Data Visualization with Power BI</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>26.66666666666667</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Machine Learning Basics</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Kafka &amp; Spark</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>SQL for Analytics</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>25</v>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>52.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>